<commit_message>
Add checked column in Reciled data sheet
</commit_message>
<xml_diff>
--- a/outputs/reconciled_data_CPRam.xlsx
+++ b/outputs/reconciled_data_CPRam.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V84"/>
+  <dimension ref="A1:AA84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,6 +545,31 @@
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
+          <t>INV.no Check</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Inv. Date Check</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>ExcludeVAT_diff</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>VAT_diff</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>IncludeVAT_diff</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
           <t>null_report</t>
         </is>
       </c>
@@ -635,7 +660,22 @@
       <c r="U2" t="n">
         <v>1867.43</v>
       </c>
-      <c r="V2" t="inlineStr"/>
+      <c r="V2" t="b">
+        <v>1</v>
+      </c>
+      <c r="W2" t="b">
+        <v>1</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -723,7 +763,22 @@
       <c r="U3" t="n">
         <v>4018.16</v>
       </c>
-      <c r="V3" t="inlineStr"/>
+      <c r="V3" t="b">
+        <v>1</v>
+      </c>
+      <c r="W3" t="b">
+        <v>1</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -811,7 +866,22 @@
       <c r="U4" t="n">
         <v>2419.06</v>
       </c>
-      <c r="V4" t="inlineStr"/>
+      <c r="V4" t="b">
+        <v>1</v>
+      </c>
+      <c r="W4" t="b">
+        <v>1</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -899,7 +969,22 @@
       <c r="U5" t="n">
         <v>2444.13</v>
       </c>
-      <c r="V5" t="inlineStr"/>
+      <c r="V5" t="b">
+        <v>1</v>
+      </c>
+      <c r="W5" t="b">
+        <v>1</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -987,7 +1072,22 @@
       <c r="U6" t="n">
         <v>2265.32</v>
       </c>
-      <c r="V6" t="inlineStr"/>
+      <c r="V6" t="b">
+        <v>1</v>
+      </c>
+      <c r="W6" t="b">
+        <v>1</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1075,7 +1175,22 @@
       <c r="U7" t="n">
         <v>4883.15</v>
       </c>
-      <c r="V7" t="inlineStr"/>
+      <c r="V7" t="b">
+        <v>1</v>
+      </c>
+      <c r="W7" t="b">
+        <v>1</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1163,7 +1278,22 @@
       <c r="U8" t="n">
         <v>8872.01</v>
       </c>
-      <c r="V8" t="inlineStr"/>
+      <c r="V8" t="b">
+        <v>1</v>
+      </c>
+      <c r="W8" t="b">
+        <v>1</v>
+      </c>
+      <c r="X8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1251,7 +1381,22 @@
       <c r="U9" t="n">
         <v>983.14</v>
       </c>
-      <c r="V9" t="inlineStr"/>
+      <c r="V9" t="b">
+        <v>1</v>
+      </c>
+      <c r="W9" t="b">
+        <v>1</v>
+      </c>
+      <c r="X9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1339,7 +1484,22 @@
       <c r="U10" t="n">
         <v>6639.34</v>
       </c>
-      <c r="V10" t="inlineStr"/>
+      <c r="V10" t="b">
+        <v>1</v>
+      </c>
+      <c r="W10" t="b">
+        <v>1</v>
+      </c>
+      <c r="X10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1427,7 +1587,22 @@
       <c r="U11" t="n">
         <v>3229.13</v>
       </c>
-      <c r="V11" t="inlineStr"/>
+      <c r="V11" t="b">
+        <v>1</v>
+      </c>
+      <c r="W11" t="b">
+        <v>1</v>
+      </c>
+      <c r="X11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1515,7 +1690,22 @@
       <c r="U12" t="n">
         <v>1493.01</v>
       </c>
-      <c r="V12" t="inlineStr"/>
+      <c r="V12" t="b">
+        <v>1</v>
+      </c>
+      <c r="W12" t="b">
+        <v>1</v>
+      </c>
+      <c r="X12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1603,7 +1793,22 @@
       <c r="U13" t="n">
         <v>1471.25</v>
       </c>
-      <c r="V13" t="inlineStr"/>
+      <c r="V13" t="b">
+        <v>1</v>
+      </c>
+      <c r="W13" t="b">
+        <v>1</v>
+      </c>
+      <c r="X13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1691,7 +1896,22 @@
       <c r="U14" t="n">
         <v>3128.02</v>
       </c>
-      <c r="V14" t="inlineStr"/>
+      <c r="V14" t="b">
+        <v>1</v>
+      </c>
+      <c r="W14" t="b">
+        <v>1</v>
+      </c>
+      <c r="X14" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1779,7 +1999,22 @@
       <c r="U15" t="n">
         <v>4045.78</v>
       </c>
-      <c r="V15" t="inlineStr"/>
+      <c r="V15" t="b">
+        <v>1</v>
+      </c>
+      <c r="W15" t="b">
+        <v>1</v>
+      </c>
+      <c r="X15" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1867,7 +2102,22 @@
       <c r="U16" t="n">
         <v>2491.5</v>
       </c>
-      <c r="V16" t="inlineStr"/>
+      <c r="V16" t="b">
+        <v>1</v>
+      </c>
+      <c r="W16" t="b">
+        <v>1</v>
+      </c>
+      <c r="X16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1955,7 +2205,22 @@
       <c r="U17" t="n">
         <v>5294.31</v>
       </c>
-      <c r="V17" t="inlineStr"/>
+      <c r="V17" t="b">
+        <v>1</v>
+      </c>
+      <c r="W17" t="b">
+        <v>1</v>
+      </c>
+      <c r="X17" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2043,7 +2308,22 @@
       <c r="U18" t="n">
         <v>2883.54</v>
       </c>
-      <c r="V18" t="inlineStr"/>
+      <c r="V18" t="b">
+        <v>1</v>
+      </c>
+      <c r="W18" t="b">
+        <v>1</v>
+      </c>
+      <c r="X18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2131,7 +2411,22 @@
       <c r="U19" t="n">
         <v>3263.5</v>
       </c>
-      <c r="V19" t="inlineStr"/>
+      <c r="V19" t="b">
+        <v>1</v>
+      </c>
+      <c r="W19" t="b">
+        <v>1</v>
+      </c>
+      <c r="X19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2219,7 +2514,22 @@
       <c r="U20" t="n">
         <v>1579.96</v>
       </c>
-      <c r="V20" t="inlineStr"/>
+      <c r="V20" t="b">
+        <v>1</v>
+      </c>
+      <c r="W20" t="b">
+        <v>1</v>
+      </c>
+      <c r="X20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2307,7 +2617,22 @@
       <c r="U21" t="n">
         <v>12483.54</v>
       </c>
-      <c r="V21" t="inlineStr"/>
+      <c r="V21" t="b">
+        <v>1</v>
+      </c>
+      <c r="W21" t="b">
+        <v>1</v>
+      </c>
+      <c r="X21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2395,7 +2720,22 @@
       <c r="U22" t="n">
         <v>1607</v>
       </c>
-      <c r="V22" t="inlineStr"/>
+      <c r="V22" t="b">
+        <v>1</v>
+      </c>
+      <c r="W22" t="b">
+        <v>1</v>
+      </c>
+      <c r="X22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2483,7 +2823,22 @@
       <c r="U23" t="n">
         <v>4751.7</v>
       </c>
-      <c r="V23" t="inlineStr"/>
+      <c r="V23" t="b">
+        <v>1</v>
+      </c>
+      <c r="W23" t="b">
+        <v>1</v>
+      </c>
+      <c r="X23" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2571,7 +2926,22 @@
       <c r="U24" t="n">
         <v>582.1</v>
       </c>
-      <c r="V24" t="inlineStr"/>
+      <c r="V24" t="b">
+        <v>1</v>
+      </c>
+      <c r="W24" t="b">
+        <v>1</v>
+      </c>
+      <c r="X24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2659,7 +3029,22 @@
       <c r="U25" t="n">
         <v>3384.62</v>
       </c>
-      <c r="V25" t="inlineStr"/>
+      <c r="V25" t="b">
+        <v>1</v>
+      </c>
+      <c r="W25" t="b">
+        <v>1</v>
+      </c>
+      <c r="X25" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2747,7 +3132,22 @@
       <c r="U26" t="n">
         <v>1714.53</v>
       </c>
-      <c r="V26" t="inlineStr"/>
+      <c r="V26" t="b">
+        <v>1</v>
+      </c>
+      <c r="W26" t="b">
+        <v>1</v>
+      </c>
+      <c r="X26" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2835,7 +3235,22 @@
       <c r="U27" t="n">
         <v>1958.71</v>
       </c>
-      <c r="V27" t="inlineStr"/>
+      <c r="V27" t="b">
+        <v>1</v>
+      </c>
+      <c r="W27" t="b">
+        <v>1</v>
+      </c>
+      <c r="X27" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2923,7 +3338,22 @@
       <c r="U28" t="n">
         <v>1659.81</v>
       </c>
-      <c r="V28" t="inlineStr"/>
+      <c r="V28" t="b">
+        <v>1</v>
+      </c>
+      <c r="W28" t="b">
+        <v>1</v>
+      </c>
+      <c r="X28" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3011,7 +3441,22 @@
       <c r="U29" t="n">
         <v>789.98</v>
       </c>
-      <c r="V29" t="inlineStr"/>
+      <c r="V29" t="b">
+        <v>1</v>
+      </c>
+      <c r="W29" t="b">
+        <v>1</v>
+      </c>
+      <c r="X29" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3099,7 +3544,22 @@
       <c r="U30" t="n">
         <v>3360.84</v>
       </c>
-      <c r="V30" t="inlineStr"/>
+      <c r="V30" t="b">
+        <v>1</v>
+      </c>
+      <c r="W30" t="b">
+        <v>1</v>
+      </c>
+      <c r="X30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3187,7 +3647,22 @@
       <c r="U31" t="n">
         <v>1659.81</v>
       </c>
-      <c r="V31" t="inlineStr"/>
+      <c r="V31" t="b">
+        <v>1</v>
+      </c>
+      <c r="W31" t="b">
+        <v>1</v>
+      </c>
+      <c r="X31" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3275,7 +3750,22 @@
       <c r="U32" t="n">
         <v>1319.53</v>
       </c>
-      <c r="V32" t="inlineStr"/>
+      <c r="V32" t="b">
+        <v>1</v>
+      </c>
+      <c r="W32" t="b">
+        <v>1</v>
+      </c>
+      <c r="X32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3363,7 +3853,22 @@
       <c r="U33" t="n">
         <v>2890.4</v>
       </c>
-      <c r="V33" t="inlineStr"/>
+      <c r="V33" t="b">
+        <v>1</v>
+      </c>
+      <c r="W33" t="b">
+        <v>1</v>
+      </c>
+      <c r="X33" t="n">
+        <v>-2.66</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>2.66</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3451,7 +3956,22 @@
       <c r="U34" t="n">
         <v>3264.93</v>
       </c>
-      <c r="V34" t="inlineStr"/>
+      <c r="V34" t="b">
+        <v>1</v>
+      </c>
+      <c r="W34" t="b">
+        <v>1</v>
+      </c>
+      <c r="X34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3539,7 +4059,22 @@
       <c r="U35" t="n">
         <v>2460.08</v>
       </c>
-      <c r="V35" t="inlineStr"/>
+      <c r="V35" t="b">
+        <v>1</v>
+      </c>
+      <c r="W35" t="b">
+        <v>1</v>
+      </c>
+      <c r="X35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3627,7 +4162,22 @@
       <c r="U36" t="n">
         <v>1768.31</v>
       </c>
-      <c r="V36" t="inlineStr"/>
+      <c r="V36" t="b">
+        <v>1</v>
+      </c>
+      <c r="W36" t="b">
+        <v>1</v>
+      </c>
+      <c r="X36" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y36" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z36" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -3715,7 +4265,22 @@
       <c r="U37" t="n">
         <v>4849.56</v>
       </c>
-      <c r="V37" t="inlineStr"/>
+      <c r="V37" t="b">
+        <v>1</v>
+      </c>
+      <c r="W37" t="b">
+        <v>1</v>
+      </c>
+      <c r="X37" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y37" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -3803,7 +4368,22 @@
       <c r="U38" t="n">
         <v>3214</v>
       </c>
-      <c r="V38" t="inlineStr"/>
+      <c r="V38" t="b">
+        <v>1</v>
+      </c>
+      <c r="W38" t="b">
+        <v>1</v>
+      </c>
+      <c r="X38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -3891,7 +4471,22 @@
       <c r="U39" t="n">
         <v>2295.63</v>
       </c>
-      <c r="V39" t="inlineStr"/>
+      <c r="V39" t="b">
+        <v>1</v>
+      </c>
+      <c r="W39" t="b">
+        <v>1</v>
+      </c>
+      <c r="X39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -3979,7 +4574,22 @@
       <c r="U40" t="n">
         <v>1169.02</v>
       </c>
-      <c r="V40" t="inlineStr"/>
+      <c r="V40" t="b">
+        <v>1</v>
+      </c>
+      <c r="W40" t="b">
+        <v>1</v>
+      </c>
+      <c r="X40" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y40" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -4067,7 +4677,22 @@
       <c r="U41" t="n">
         <v>4095.55</v>
       </c>
-      <c r="V41" t="inlineStr"/>
+      <c r="V41" t="b">
+        <v>1</v>
+      </c>
+      <c r="W41" t="b">
+        <v>1</v>
+      </c>
+      <c r="X41" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y41" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -4155,7 +4780,22 @@
       <c r="U42" t="n">
         <v>2519.38</v>
       </c>
-      <c r="V42" t="inlineStr"/>
+      <c r="V42" t="b">
+        <v>1</v>
+      </c>
+      <c r="W42" t="b">
+        <v>1</v>
+      </c>
+      <c r="X42" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y42" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z42" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -4243,7 +4883,22 @@
       <c r="U43" t="n">
         <v>4951.2</v>
       </c>
-      <c r="V43" t="inlineStr"/>
+      <c r="V43" t="b">
+        <v>1</v>
+      </c>
+      <c r="W43" t="b">
+        <v>1</v>
+      </c>
+      <c r="X43" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y43" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z43" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -4331,7 +4986,22 @@
       <c r="U44" t="n">
         <v>2405.51</v>
       </c>
-      <c r="V44" t="inlineStr"/>
+      <c r="V44" t="b">
+        <v>1</v>
+      </c>
+      <c r="W44" t="b">
+        <v>1</v>
+      </c>
+      <c r="X44" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y44" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z44" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -4419,7 +5089,22 @@
       <c r="U45" t="n">
         <v>2358.68</v>
       </c>
-      <c r="V45" t="inlineStr"/>
+      <c r="V45" t="b">
+        <v>1</v>
+      </c>
+      <c r="W45" t="b">
+        <v>1</v>
+      </c>
+      <c r="X45" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y45" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -4507,7 +5192,22 @@
       <c r="U46" t="n">
         <v>2732.74</v>
       </c>
-      <c r="V46" t="inlineStr"/>
+      <c r="V46" t="b">
+        <v>1</v>
+      </c>
+      <c r="W46" t="b">
+        <v>1</v>
+      </c>
+      <c r="X46" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y46" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z46" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -4595,7 +5295,22 @@
       <c r="U47" t="n">
         <v>1877.79</v>
       </c>
-      <c r="V47" t="inlineStr"/>
+      <c r="V47" t="b">
+        <v>1</v>
+      </c>
+      <c r="W47" t="b">
+        <v>1</v>
+      </c>
+      <c r="X47" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y47" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -4683,7 +5398,22 @@
       <c r="U48" t="n">
         <v>3477.09</v>
       </c>
-      <c r="V48" t="inlineStr"/>
+      <c r="V48" t="b">
+        <v>1</v>
+      </c>
+      <c r="W48" t="b">
+        <v>1</v>
+      </c>
+      <c r="X48" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y48" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -4771,7 +5501,22 @@
       <c r="U49" t="n">
         <v>1607</v>
       </c>
-      <c r="V49" t="inlineStr"/>
+      <c r="V49" t="b">
+        <v>1</v>
+      </c>
+      <c r="W49" t="b">
+        <v>1</v>
+      </c>
+      <c r="X49" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y49" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z49" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -4859,7 +5604,22 @@
       <c r="U50" t="n">
         <v>2332.79</v>
       </c>
-      <c r="V50" t="inlineStr"/>
+      <c r="V50" t="b">
+        <v>1</v>
+      </c>
+      <c r="W50" t="b">
+        <v>1</v>
+      </c>
+      <c r="X50" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y50" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z50" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -4947,7 +5707,22 @@
       <c r="U51" t="n">
         <v>1579.96</v>
       </c>
-      <c r="V51" t="inlineStr"/>
+      <c r="V51" t="b">
+        <v>1</v>
+      </c>
+      <c r="W51" t="b">
+        <v>1</v>
+      </c>
+      <c r="X51" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y51" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z51" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -5035,7 +5810,22 @@
       <c r="U52" t="n">
         <v>1564.01</v>
       </c>
-      <c r="V52" t="inlineStr"/>
+      <c r="V52" t="b">
+        <v>1</v>
+      </c>
+      <c r="W52" t="b">
+        <v>1</v>
+      </c>
+      <c r="X52" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y52" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z52" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -5123,7 +5913,22 @@
       <c r="U53" t="n">
         <v>669.58</v>
       </c>
-      <c r="V53" t="inlineStr"/>
+      <c r="V53" t="b">
+        <v>1</v>
+      </c>
+      <c r="W53" t="b">
+        <v>1</v>
+      </c>
+      <c r="X53" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y53" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z53" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -5211,7 +6016,22 @@
       <c r="U54" t="n">
         <v>4618.71</v>
       </c>
-      <c r="V54" t="inlineStr"/>
+      <c r="V54" t="b">
+        <v>1</v>
+      </c>
+      <c r="W54" t="b">
+        <v>1</v>
+      </c>
+      <c r="X54" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y54" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z54" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -5299,7 +6119,22 @@
       <c r="U55" t="n">
         <v>8106.14</v>
       </c>
-      <c r="V55" t="inlineStr"/>
+      <c r="V55" t="b">
+        <v>1</v>
+      </c>
+      <c r="W55" t="b">
+        <v>1</v>
+      </c>
+      <c r="X55" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y55" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -5387,7 +6222,22 @@
       <c r="U56" t="n">
         <v>157.66</v>
       </c>
-      <c r="V56" t="inlineStr"/>
+      <c r="V56" t="b">
+        <v>1</v>
+      </c>
+      <c r="W56" t="b">
+        <v>1</v>
+      </c>
+      <c r="X56" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y56" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -5475,7 +6325,22 @@
       <c r="U57" t="n">
         <v>2060.11</v>
       </c>
-      <c r="V57" t="inlineStr"/>
+      <c r="V57" t="b">
+        <v>1</v>
+      </c>
+      <c r="W57" t="b">
+        <v>1</v>
+      </c>
+      <c r="X57" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y57" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z57" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -5563,7 +6428,22 @@
       <c r="U58" t="n">
         <v>1184.97</v>
       </c>
-      <c r="V58" t="inlineStr"/>
+      <c r="V58" t="b">
+        <v>1</v>
+      </c>
+      <c r="W58" t="b">
+        <v>1</v>
+      </c>
+      <c r="X58" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y58" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z58" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -5651,7 +6531,22 @@
       <c r="U59" t="n">
         <v>2109.52</v>
       </c>
-      <c r="V59" t="inlineStr"/>
+      <c r="V59" t="b">
+        <v>1</v>
+      </c>
+      <c r="W59" t="b">
+        <v>1</v>
+      </c>
+      <c r="X59" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y59" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -5739,7 +6634,22 @@
       <c r="U60" t="n">
         <v>3100.1</v>
       </c>
-      <c r="V60" t="inlineStr"/>
+      <c r="V60" t="b">
+        <v>1</v>
+      </c>
+      <c r="W60" t="b">
+        <v>1</v>
+      </c>
+      <c r="X60" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y60" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z60" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -5827,7 +6737,22 @@
       <c r="U61" t="n">
         <v>1530.56</v>
       </c>
-      <c r="V61" t="inlineStr"/>
+      <c r="V61" t="b">
+        <v>1</v>
+      </c>
+      <c r="W61" t="b">
+        <v>1</v>
+      </c>
+      <c r="X61" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y61" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z61" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -5915,7 +6840,22 @@
       <c r="U62" t="n">
         <v>2302.67</v>
       </c>
-      <c r="V62" t="inlineStr"/>
+      <c r="V62" t="b">
+        <v>1</v>
+      </c>
+      <c r="W62" t="b">
+        <v>1</v>
+      </c>
+      <c r="X62" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y62" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -6003,7 +6943,22 @@
       <c r="U63" t="n">
         <v>682.46</v>
       </c>
-      <c r="V63" t="inlineStr"/>
+      <c r="V63" t="b">
+        <v>1</v>
+      </c>
+      <c r="W63" t="b">
+        <v>1</v>
+      </c>
+      <c r="X63" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y63" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z63" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -6091,7 +7046,22 @@
       <c r="U64" t="n">
         <v>2706.52</v>
       </c>
-      <c r="V64" t="inlineStr"/>
+      <c r="V64" t="b">
+        <v>1</v>
+      </c>
+      <c r="W64" t="b">
+        <v>1</v>
+      </c>
+      <c r="X64" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y64" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z64" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -6179,7 +7149,22 @@
       <c r="U65" t="n">
         <v>2483.03</v>
       </c>
-      <c r="V65" t="inlineStr"/>
+      <c r="V65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W65" t="b">
+        <v>1</v>
+      </c>
+      <c r="X65" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y65" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z65" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -6267,7 +7252,22 @@
       <c r="U66" t="n">
         <v>6444.9</v>
       </c>
-      <c r="V66" t="inlineStr"/>
+      <c r="V66" t="b">
+        <v>1</v>
+      </c>
+      <c r="W66" t="b">
+        <v>1</v>
+      </c>
+      <c r="X66" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y66" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -6355,7 +7355,22 @@
       <c r="U67" t="n">
         <v>365.11</v>
       </c>
-      <c r="V67" t="inlineStr"/>
+      <c r="V67" t="b">
+        <v>1</v>
+      </c>
+      <c r="W67" t="b">
+        <v>1</v>
+      </c>
+      <c r="X67" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y67" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -6443,7 +7458,22 @@
       <c r="U68" t="n">
         <v>275.3</v>
       </c>
-      <c r="V68" t="inlineStr"/>
+      <c r="V68" t="b">
+        <v>1</v>
+      </c>
+      <c r="W68" t="b">
+        <v>1</v>
+      </c>
+      <c r="X68" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y68" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z68" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -6531,7 +7561,22 @@
       <c r="U69" t="n">
         <v>2972.36</v>
       </c>
-      <c r="V69" t="inlineStr"/>
+      <c r="V69" t="b">
+        <v>1</v>
+      </c>
+      <c r="W69" t="b">
+        <v>1</v>
+      </c>
+      <c r="X69" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y69" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z69" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -6587,7 +7632,16 @@
       <c r="S70" t="inlineStr"/>
       <c r="T70" t="inlineStr"/>
       <c r="U70" t="inlineStr"/>
-      <c r="V70" t="inlineStr">
+      <c r="V70" t="b">
+        <v>0</v>
+      </c>
+      <c r="W70" t="b">
+        <v>0</v>
+      </c>
+      <c r="X70" t="inlineStr"/>
+      <c r="Y70" t="inlineStr"/>
+      <c r="Z70" t="inlineStr"/>
+      <c r="AA70" t="inlineStr">
         <is>
           <t>CPFM_Null</t>
         </is>
@@ -6647,7 +7701,16 @@
       <c r="S71" t="inlineStr"/>
       <c r="T71" t="inlineStr"/>
       <c r="U71" t="inlineStr"/>
-      <c r="V71" t="inlineStr">
+      <c r="V71" t="b">
+        <v>0</v>
+      </c>
+      <c r="W71" t="b">
+        <v>0</v>
+      </c>
+      <c r="X71" t="inlineStr"/>
+      <c r="Y71" t="inlineStr"/>
+      <c r="Z71" t="inlineStr"/>
+      <c r="AA71" t="inlineStr">
         <is>
           <t>CPFM_Null</t>
         </is>
@@ -6707,7 +7770,16 @@
       <c r="S72" t="inlineStr"/>
       <c r="T72" t="inlineStr"/>
       <c r="U72" t="inlineStr"/>
-      <c r="V72" t="inlineStr">
+      <c r="V72" t="b">
+        <v>0</v>
+      </c>
+      <c r="W72" t="b">
+        <v>0</v>
+      </c>
+      <c r="X72" t="inlineStr"/>
+      <c r="Y72" t="inlineStr"/>
+      <c r="Z72" t="inlineStr"/>
+      <c r="AA72" t="inlineStr">
         <is>
           <t>CPFM_Null</t>
         </is>
@@ -6767,7 +7839,16 @@
       <c r="S73" t="inlineStr"/>
       <c r="T73" t="inlineStr"/>
       <c r="U73" t="inlineStr"/>
-      <c r="V73" t="inlineStr">
+      <c r="V73" t="b">
+        <v>0</v>
+      </c>
+      <c r="W73" t="b">
+        <v>0</v>
+      </c>
+      <c r="X73" t="inlineStr"/>
+      <c r="Y73" t="inlineStr"/>
+      <c r="Z73" t="inlineStr"/>
+      <c r="AA73" t="inlineStr">
         <is>
           <t>CPFM_Null</t>
         </is>
@@ -6827,7 +7908,16 @@
       <c r="S74" t="inlineStr"/>
       <c r="T74" t="inlineStr"/>
       <c r="U74" t="inlineStr"/>
-      <c r="V74" t="inlineStr">
+      <c r="V74" t="b">
+        <v>0</v>
+      </c>
+      <c r="W74" t="b">
+        <v>0</v>
+      </c>
+      <c r="X74" t="inlineStr"/>
+      <c r="Y74" t="inlineStr"/>
+      <c r="Z74" t="inlineStr"/>
+      <c r="AA74" t="inlineStr">
         <is>
           <t>CPFM_Null</t>
         </is>
@@ -6891,7 +7981,16 @@
       <c r="U75" t="n">
         <v>4132.4</v>
       </c>
-      <c r="V75" t="inlineStr">
+      <c r="V75" t="b">
+        <v>0</v>
+      </c>
+      <c r="W75" t="b">
+        <v>0</v>
+      </c>
+      <c r="X75" t="inlineStr"/>
+      <c r="Y75" t="inlineStr"/>
+      <c r="Z75" t="inlineStr"/>
+      <c r="AA75" t="inlineStr">
         <is>
           <t>BASE_Null</t>
         </is>
@@ -6955,7 +8054,16 @@
       <c r="U76" t="n">
         <v>4796.06</v>
       </c>
-      <c r="V76" t="inlineStr">
+      <c r="V76" t="b">
+        <v>0</v>
+      </c>
+      <c r="W76" t="b">
+        <v>0</v>
+      </c>
+      <c r="X76" t="inlineStr"/>
+      <c r="Y76" t="inlineStr"/>
+      <c r="Z76" t="inlineStr"/>
+      <c r="AA76" t="inlineStr">
         <is>
           <t>BASE_Null</t>
         </is>
@@ -7019,7 +8127,16 @@
       <c r="U77" t="n">
         <v>3268.32</v>
       </c>
-      <c r="V77" t="inlineStr">
+      <c r="V77" t="b">
+        <v>0</v>
+      </c>
+      <c r="W77" t="b">
+        <v>0</v>
+      </c>
+      <c r="X77" t="inlineStr"/>
+      <c r="Y77" t="inlineStr"/>
+      <c r="Z77" t="inlineStr"/>
+      <c r="AA77" t="inlineStr">
         <is>
           <t>BASE_Null</t>
         </is>
@@ -7083,7 +8200,16 @@
       <c r="U78" t="n">
         <v>1437.97</v>
       </c>
-      <c r="V78" t="inlineStr">
+      <c r="V78" t="b">
+        <v>0</v>
+      </c>
+      <c r="W78" t="b">
+        <v>0</v>
+      </c>
+      <c r="X78" t="inlineStr"/>
+      <c r="Y78" t="inlineStr"/>
+      <c r="Z78" t="inlineStr"/>
+      <c r="AA78" t="inlineStr">
         <is>
           <t>BASE_Null</t>
         </is>
@@ -7147,7 +8273,16 @@
       <c r="U79" t="n">
         <v>5889.31</v>
       </c>
-      <c r="V79" t="inlineStr">
+      <c r="V79" t="b">
+        <v>0</v>
+      </c>
+      <c r="W79" t="b">
+        <v>0</v>
+      </c>
+      <c r="X79" t="inlineStr"/>
+      <c r="Y79" t="inlineStr"/>
+      <c r="Z79" t="inlineStr"/>
+      <c r="AA79" t="inlineStr">
         <is>
           <t>BASE_Null</t>
         </is>
@@ -7211,7 +8346,16 @@
       <c r="U80" t="n">
         <v>5036.9</v>
       </c>
-      <c r="V80" t="inlineStr">
+      <c r="V80" t="b">
+        <v>0</v>
+      </c>
+      <c r="W80" t="b">
+        <v>0</v>
+      </c>
+      <c r="X80" t="inlineStr"/>
+      <c r="Y80" t="inlineStr"/>
+      <c r="Z80" t="inlineStr"/>
+      <c r="AA80" t="inlineStr">
         <is>
           <t>BASE_Null</t>
         </is>
@@ -7275,7 +8419,16 @@
       <c r="U81" t="n">
         <v>614.05</v>
       </c>
-      <c r="V81" t="inlineStr">
+      <c r="V81" t="b">
+        <v>0</v>
+      </c>
+      <c r="W81" t="b">
+        <v>0</v>
+      </c>
+      <c r="X81" t="inlineStr"/>
+      <c r="Y81" t="inlineStr"/>
+      <c r="Z81" t="inlineStr"/>
+      <c r="AA81" t="inlineStr">
         <is>
           <t>BASE_Null</t>
         </is>
@@ -7339,7 +8492,16 @@
       <c r="U82" t="n">
         <v>1312.31</v>
       </c>
-      <c r="V82" t="inlineStr">
+      <c r="V82" t="b">
+        <v>0</v>
+      </c>
+      <c r="W82" t="b">
+        <v>0</v>
+      </c>
+      <c r="X82" t="inlineStr"/>
+      <c r="Y82" t="inlineStr"/>
+      <c r="Z82" t="inlineStr"/>
+      <c r="AA82" t="inlineStr">
         <is>
           <t>BASE_Null</t>
         </is>
@@ -7403,7 +8565,16 @@
       <c r="U83" t="n">
         <v>3929.08</v>
       </c>
-      <c r="V83" t="inlineStr">
+      <c r="V83" t="b">
+        <v>0</v>
+      </c>
+      <c r="W83" t="b">
+        <v>0</v>
+      </c>
+      <c r="X83" t="inlineStr"/>
+      <c r="Y83" t="inlineStr"/>
+      <c r="Z83" t="inlineStr"/>
+      <c r="AA83" t="inlineStr">
         <is>
           <t>BASE_Null</t>
         </is>
@@ -7467,7 +8638,16 @@
       <c r="U84" t="n">
         <v>4012.36</v>
       </c>
-      <c r="V84" t="inlineStr">
+      <c r="V84" t="b">
+        <v>0</v>
+      </c>
+      <c r="W84" t="b">
+        <v>0</v>
+      </c>
+      <c r="X84" t="inlineStr"/>
+      <c r="Y84" t="inlineStr"/>
+      <c r="Z84" t="inlineStr"/>
+      <c r="AA84" t="inlineStr">
         <is>
           <t>BASE_Null</t>
         </is>
@@ -8145,7 +9325,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V11"/>
+  <dimension ref="A1:AA11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8260,6 +9440,31 @@
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>INV.no Check</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Inv. Date Check</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>ExcludeVAT_diff</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>VAT_diff</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>IncludeVAT_diff</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>null_report</t>
         </is>
@@ -8323,7 +9528,16 @@
       <c r="U2" t="n">
         <v>4132.4</v>
       </c>
-      <c r="V2" t="inlineStr">
+      <c r="V2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W2" t="b">
+        <v>0</v>
+      </c>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr">
         <is>
           <t>BASE_Null</t>
         </is>
@@ -8387,7 +9601,16 @@
       <c r="U3" t="n">
         <v>4796.06</v>
       </c>
-      <c r="V3" t="inlineStr">
+      <c r="V3" t="b">
+        <v>0</v>
+      </c>
+      <c r="W3" t="b">
+        <v>0</v>
+      </c>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr">
         <is>
           <t>BASE_Null</t>
         </is>
@@ -8451,7 +9674,16 @@
       <c r="U4" t="n">
         <v>3268.32</v>
       </c>
-      <c r="V4" t="inlineStr">
+      <c r="V4" t="b">
+        <v>0</v>
+      </c>
+      <c r="W4" t="b">
+        <v>0</v>
+      </c>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr">
         <is>
           <t>BASE_Null</t>
         </is>
@@ -8515,7 +9747,16 @@
       <c r="U5" t="n">
         <v>1437.97</v>
       </c>
-      <c r="V5" t="inlineStr">
+      <c r="V5" t="b">
+        <v>0</v>
+      </c>
+      <c r="W5" t="b">
+        <v>0</v>
+      </c>
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="inlineStr">
         <is>
           <t>BASE_Null</t>
         </is>
@@ -8579,7 +9820,16 @@
       <c r="U6" t="n">
         <v>5889.31</v>
       </c>
-      <c r="V6" t="inlineStr">
+      <c r="V6" t="b">
+        <v>0</v>
+      </c>
+      <c r="W6" t="b">
+        <v>0</v>
+      </c>
+      <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr"/>
+      <c r="AA6" t="inlineStr">
         <is>
           <t>BASE_Null</t>
         </is>
@@ -8643,7 +9893,16 @@
       <c r="U7" t="n">
         <v>5036.9</v>
       </c>
-      <c r="V7" t="inlineStr">
+      <c r="V7" t="b">
+        <v>0</v>
+      </c>
+      <c r="W7" t="b">
+        <v>0</v>
+      </c>
+      <c r="X7" t="inlineStr"/>
+      <c r="Y7" t="inlineStr"/>
+      <c r="Z7" t="inlineStr"/>
+      <c r="AA7" t="inlineStr">
         <is>
           <t>BASE_Null</t>
         </is>
@@ -8707,7 +9966,16 @@
       <c r="U8" t="n">
         <v>614.05</v>
       </c>
-      <c r="V8" t="inlineStr">
+      <c r="V8" t="b">
+        <v>0</v>
+      </c>
+      <c r="W8" t="b">
+        <v>0</v>
+      </c>
+      <c r="X8" t="inlineStr"/>
+      <c r="Y8" t="inlineStr"/>
+      <c r="Z8" t="inlineStr"/>
+      <c r="AA8" t="inlineStr">
         <is>
           <t>BASE_Null</t>
         </is>
@@ -8771,7 +10039,16 @@
       <c r="U9" t="n">
         <v>1312.31</v>
       </c>
-      <c r="V9" t="inlineStr">
+      <c r="V9" t="b">
+        <v>0</v>
+      </c>
+      <c r="W9" t="b">
+        <v>0</v>
+      </c>
+      <c r="X9" t="inlineStr"/>
+      <c r="Y9" t="inlineStr"/>
+      <c r="Z9" t="inlineStr"/>
+      <c r="AA9" t="inlineStr">
         <is>
           <t>BASE_Null</t>
         </is>
@@ -8835,7 +10112,16 @@
       <c r="U10" t="n">
         <v>3929.08</v>
       </c>
-      <c r="V10" t="inlineStr">
+      <c r="V10" t="b">
+        <v>0</v>
+      </c>
+      <c r="W10" t="b">
+        <v>0</v>
+      </c>
+      <c r="X10" t="inlineStr"/>
+      <c r="Y10" t="inlineStr"/>
+      <c r="Z10" t="inlineStr"/>
+      <c r="AA10" t="inlineStr">
         <is>
           <t>BASE_Null</t>
         </is>
@@ -8899,7 +10185,16 @@
       <c r="U11" t="n">
         <v>4012.36</v>
       </c>
-      <c r="V11" t="inlineStr">
+      <c r="V11" t="b">
+        <v>0</v>
+      </c>
+      <c r="W11" t="b">
+        <v>0</v>
+      </c>
+      <c r="X11" t="inlineStr"/>
+      <c r="Y11" t="inlineStr"/>
+      <c r="Z11" t="inlineStr"/>
+      <c r="AA11" t="inlineStr">
         <is>
           <t>BASE_Null</t>
         </is>
@@ -8916,7 +10211,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9031,6 +10326,31 @@
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>INV.no Check</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Inv. Date Check</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>ExcludeVAT_diff</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>VAT_diff</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>IncludeVAT_diff</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>null_report</t>
         </is>
@@ -9090,7 +10410,16 @@
       <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr"/>
       <c r="U2" t="inlineStr"/>
-      <c r="V2" t="inlineStr">
+      <c r="V2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W2" t="b">
+        <v>0</v>
+      </c>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr">
         <is>
           <t>CPFM_Null</t>
         </is>
@@ -9150,7 +10479,16 @@
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr"/>
-      <c r="V3" t="inlineStr">
+      <c r="V3" t="b">
+        <v>0</v>
+      </c>
+      <c r="W3" t="b">
+        <v>0</v>
+      </c>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr">
         <is>
           <t>CPFM_Null</t>
         </is>
@@ -9210,7 +10548,16 @@
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
       <c r="U4" t="inlineStr"/>
-      <c r="V4" t="inlineStr">
+      <c r="V4" t="b">
+        <v>0</v>
+      </c>
+      <c r="W4" t="b">
+        <v>0</v>
+      </c>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr">
         <is>
           <t>CPFM_Null</t>
         </is>
@@ -9270,7 +10617,16 @@
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
       <c r="U5" t="inlineStr"/>
-      <c r="V5" t="inlineStr">
+      <c r="V5" t="b">
+        <v>0</v>
+      </c>
+      <c r="W5" t="b">
+        <v>0</v>
+      </c>
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="inlineStr">
         <is>
           <t>CPFM_Null</t>
         </is>
@@ -9330,7 +10686,16 @@
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
       <c r="U6" t="inlineStr"/>
-      <c r="V6" t="inlineStr">
+      <c r="V6" t="b">
+        <v>0</v>
+      </c>
+      <c r="W6" t="b">
+        <v>0</v>
+      </c>
+      <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr"/>
+      <c r="AA6" t="inlineStr">
         <is>
           <t>CPFM_Null</t>
         </is>
@@ -9347,7 +10712,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9378,31 +10743,21 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DIFF</t>
+          <t>Matching</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Matching</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>